<commit_message>
removing an extra file
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -426,9 +426,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.875" collapsed="false"/>
-    <col min="2" max="3" customWidth="true" width="13.625" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="10.875" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="16.875" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="13.625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>